<commit_message>
Se agrego casos de pruebas funcionales.xlsx y se modifico el index para que muestre avatar e imagen de inicio
</commit_message>
<xml_diff>
--- a/Casos pruebas funcionales.xlsx
+++ b/Casos pruebas funcionales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\cirv8\Documents\MEGA\Cursos\CoderHouse\Python\Clase 24 - Playground Avanzado parte III\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\proyecto_final_blog\proyecto_blog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235BE547-484A-4E60-95C6-5BB91DFA70F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD4956F-1D85-4BB8-926F-BBD2465D368F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Solo se pueden eliminar los articulos creados por el usuario.</t>
+  </si>
+  <si>
+    <t>Dirige a la página de inicio y muestra mensaje de Bienvenida + nombre de usuario y avatar por defecto ademas en el nombre de usuario del panel de navegacion aparece avatar por defecto</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
   <dimension ref="A1:Y1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -656,7 +659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="36" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>1</v>
       </c>
@@ -745,7 +748,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>27</v>

</xml_diff>